<commit_message>
new twitter social analysis (engage vs museum tweets)
</commit_message>
<xml_diff>
--- a/data/analysis/missing_web_soc_museums/missing_web_soc_museum_wide_pc.xlsx
+++ b/data/analysis/missing_web_soc_museums/missing_web_soc_museum_wide_pc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="173">
   <si>
     <t>var1_name</t>
   </si>
@@ -52,6 +52,9 @@
     <t>subject_matter</t>
   </si>
   <si>
+    <t>subject_matter_simpl</t>
+  </si>
+  <si>
     <t>Accredited</t>
   </si>
   <si>
@@ -479,6 +482,57 @@
   </si>
   <si>
     <t>War and conflict:Regiment</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>Belief and identity</t>
+  </si>
+  <si>
+    <t>Buildings</t>
+  </si>
+  <si>
+    <t>Communications</t>
+  </si>
+  <si>
+    <t>Industry and manufacture</t>
+  </si>
+  <si>
+    <t>Leisure and sport</t>
+  </si>
+  <si>
+    <t>Medicine and health</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Natural world</t>
+  </si>
+  <si>
+    <t>Personality</t>
+  </si>
+  <si>
+    <t>Rural Industry</t>
+  </si>
+  <si>
+    <t>Science and technology</t>
+  </si>
+  <si>
+    <t>Sea and seafaring</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>War and conflict</t>
   </si>
 </sst>
 </file>
@@ -836,7 +890,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:F166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -867,13 +921,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>14.2</v>
+        <v>17.8</v>
       </c>
       <c r="D2">
-        <v>20.5</v>
+        <v>24.2</v>
       </c>
       <c r="E2">
         <v>0.3</v>
@@ -887,13 +941,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>25.1</v>
+        <v>29.1</v>
       </c>
       <c r="D3">
-        <v>38.3</v>
+        <v>42.2</v>
       </c>
       <c r="E3">
         <v>1.8</v>
@@ -907,13 +961,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>33.3</v>
+        <v>100</v>
       </c>
       <c r="D4">
-        <v>33.3</v>
+        <v>100</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -927,13 +981,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>16.5</v>
+        <v>24.4</v>
       </c>
       <c r="D5">
-        <v>24.4</v>
+        <v>31.8</v>
       </c>
       <c r="E5">
         <v>0.1</v>
@@ -947,13 +1001,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>17.4</v>
+        <v>18.8</v>
       </c>
       <c r="D6">
-        <v>15.9</v>
+        <v>20.3</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -967,7 +1021,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -987,10 +1041,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>30.8</v>
+        <v>32.7</v>
       </c>
       <c r="D8">
         <v>55.8</v>
@@ -1007,13 +1061,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>73.7</v>
       </c>
       <c r="D9">
-        <v>89.5</v>
+        <v>94.7</v>
       </c>
       <c r="E9">
         <v>5.3</v>
@@ -1027,10 +1081,10 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>12.6</v>
       </c>
       <c r="D10">
         <v>21.9</v>
@@ -1047,7 +1101,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>11.5</v>
@@ -1067,13 +1121,13 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D12">
-        <v>27.9</v>
+        <v>30.3</v>
       </c>
       <c r="E12">
         <v>0.8</v>
@@ -1087,13 +1141,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13">
-        <v>24.7</v>
+        <v>29.2</v>
       </c>
       <c r="D13">
-        <v>37.6</v>
+        <v>40.6</v>
       </c>
       <c r="E13">
         <v>2.6</v>
@@ -1107,13 +1161,13 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14">
-        <v>29.7</v>
+        <v>33.3</v>
       </c>
       <c r="D14">
-        <v>50.5</v>
+        <v>55</v>
       </c>
       <c r="E14">
         <v>4.5</v>
@@ -1127,13 +1181,13 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15">
         <v>25</v>
       </c>
-      <c r="C15">
-        <v>15.2</v>
-      </c>
       <c r="D15">
-        <v>9.800000000000001</v>
+        <v>18.5</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1147,13 +1201,13 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C16">
-        <v>25.5</v>
+        <v>29.1</v>
       </c>
       <c r="D16">
-        <v>54.5</v>
+        <v>58.2</v>
       </c>
       <c r="E16">
         <v>7.3</v>
@@ -1167,13 +1221,13 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17">
-        <v>16.6</v>
+        <v>24.2</v>
       </c>
       <c r="D17">
-        <v>23.8</v>
+        <v>31.1</v>
       </c>
       <c r="E17">
         <v>0.1</v>
@@ -1187,13 +1241,13 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18">
-        <v>20.7</v>
+        <v>23.1</v>
       </c>
       <c r="D18">
-        <v>31.5</v>
+        <v>33.9</v>
       </c>
       <c r="E18">
         <v>1.3</v>
@@ -1207,13 +1261,13 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19">
-        <v>15.2</v>
+        <v>25</v>
       </c>
       <c r="D19">
-        <v>9.800000000000001</v>
+        <v>18.5</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1227,13 +1281,13 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C20">
-        <v>25.5</v>
+        <v>29.1</v>
       </c>
       <c r="D20">
-        <v>54.5</v>
+        <v>58.2</v>
       </c>
       <c r="E20">
         <v>7.3</v>
@@ -1247,13 +1301,13 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C21">
-        <v>16.7</v>
+        <v>25</v>
       </c>
       <c r="D21">
-        <v>8.300000000000001</v>
+        <v>25</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1267,13 +1321,13 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C22">
-        <v>9.6</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>12.4</v>
+        <v>13.5</v>
       </c>
       <c r="E22">
         <v>0.4</v>
@@ -1287,13 +1341,13 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C23">
-        <v>14.4</v>
+        <v>19.4</v>
       </c>
       <c r="D23">
-        <v>21.4</v>
+        <v>26.6</v>
       </c>
       <c r="E23">
         <v>0.2</v>
@@ -1307,13 +1361,13 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C24">
-        <v>24.6</v>
+        <v>28.4</v>
       </c>
       <c r="D24">
-        <v>37.3</v>
+        <v>41.1</v>
       </c>
       <c r="E24">
         <v>1.6</v>
@@ -1327,13 +1381,13 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>29.3</v>
       </c>
       <c r="D25">
-        <v>40</v>
+        <v>43.6</v>
       </c>
       <c r="E25">
         <v>1.4</v>
@@ -1347,7 +1401,7 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C26">
         <v>58.3</v>
@@ -1367,13 +1421,13 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27">
-        <v>20.2</v>
+        <v>23.7</v>
       </c>
       <c r="D27">
-        <v>28.1</v>
+        <v>30.7</v>
       </c>
       <c r="E27">
         <v>0.4</v>
@@ -1387,13 +1441,13 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C28">
-        <v>21.9</v>
+        <v>24.3</v>
       </c>
       <c r="D28">
-        <v>29.4</v>
+        <v>32.7</v>
       </c>
       <c r="E28">
         <v>1.5</v>
@@ -1407,7 +1461,7 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C29">
         <v>53.3</v>
@@ -1427,13 +1481,13 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C30">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D30">
-        <v>14.7</v>
+        <v>21.8</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1447,13 +1501,13 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C31">
-        <v>19</v>
+        <v>23.8</v>
       </c>
       <c r="D31">
-        <v>25.7</v>
+        <v>31.4</v>
       </c>
       <c r="E31">
         <v>1.9</v>
@@ -1467,13 +1521,13 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C32">
-        <v>14.2</v>
+        <v>19.8</v>
       </c>
       <c r="D32">
-        <v>20.6</v>
+        <v>26.7</v>
       </c>
       <c r="E32">
         <v>0.8</v>
@@ -1487,13 +1541,13 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C33">
-        <v>19.1</v>
+        <v>27.7</v>
       </c>
       <c r="D33">
-        <v>38.3</v>
+        <v>47.9</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1507,13 +1561,13 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C34">
-        <v>24.5</v>
+        <v>27.7</v>
       </c>
       <c r="D34">
-        <v>41.1</v>
+        <v>44.1</v>
       </c>
       <c r="E34">
         <v>1.6</v>
@@ -1527,13 +1581,13 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C35">
-        <v>18.5</v>
+        <v>20.8</v>
       </c>
       <c r="D35">
-        <v>23.6</v>
+        <v>26.1</v>
       </c>
       <c r="E35">
         <v>0.6</v>
@@ -1547,13 +1601,13 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C36">
-        <v>18.6</v>
+        <v>20.5</v>
       </c>
       <c r="D36">
-        <v>31.4</v>
+        <v>33.1</v>
       </c>
       <c r="E36">
         <v>0.5</v>
@@ -1567,13 +1621,13 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C37">
-        <v>19.2</v>
+        <v>27.1</v>
       </c>
       <c r="D37">
-        <v>29.1</v>
+        <v>36</v>
       </c>
       <c r="E37">
         <v>3.4</v>
@@ -1587,13 +1641,13 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C38">
-        <v>21.5</v>
+        <v>25</v>
       </c>
       <c r="D38">
-        <v>32</v>
+        <v>37.3</v>
       </c>
       <c r="E38">
         <v>2.2</v>
@@ -1607,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C39">
-        <v>15.5</v>
+        <v>18.6</v>
       </c>
       <c r="D39">
-        <v>28.3</v>
+        <v>28.8</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1627,7 +1681,7 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1647,13 +1701,13 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C41">
-        <v>18.2</v>
+        <v>27.3</v>
       </c>
       <c r="D41">
-        <v>45.5</v>
+        <v>54.5</v>
       </c>
       <c r="E41">
         <v>9.1</v>
@@ -1667,7 +1721,7 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C42">
         <v>26.7</v>
@@ -1687,7 +1741,7 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1707,10 +1761,10 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C44">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D44">
         <v>35</v>
@@ -1727,13 +1781,13 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C45">
-        <v>21.6</v>
+        <v>27</v>
       </c>
       <c r="D45">
-        <v>29.7</v>
+        <v>35.1</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1747,10 +1801,10 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C46">
-        <v>13.3</v>
+        <v>20</v>
       </c>
       <c r="D46">
         <v>40</v>
@@ -1767,13 +1821,13 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C47">
+        <v>38.5</v>
+      </c>
+      <c r="D47">
         <v>30.8</v>
-      </c>
-      <c r="D47">
-        <v>23.1</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1787,7 +1841,7 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C48">
         <v>60</v>
@@ -1807,7 +1861,7 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C49">
         <v>25</v>
@@ -1827,13 +1881,13 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C50">
-        <v>13</v>
+        <v>16.8</v>
       </c>
       <c r="D50">
-        <v>14.9</v>
+        <v>19.3</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -1847,7 +1901,7 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C51">
         <v>40</v>
@@ -1867,13 +1921,13 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>16.7</v>
       </c>
       <c r="D52">
-        <v>33.3</v>
+        <v>50</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -1887,13 +1941,13 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C53">
+        <v>25</v>
+      </c>
+      <c r="D53">
         <v>18.8</v>
-      </c>
-      <c r="D53">
-        <v>12.5</v>
       </c>
       <c r="E53">
         <v>6.2</v>
@@ -1907,7 +1961,7 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C54">
         <v>23.1</v>
@@ -1927,7 +1981,7 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C55">
         <v>33.3</v>
@@ -1947,13 +2001,13 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C56">
-        <v>28.6</v>
+        <v>42.9</v>
       </c>
       <c r="D56">
-        <v>28.6</v>
+        <v>42.9</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -1967,13 +2021,13 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C57">
-        <v>31.2</v>
+        <v>37.5</v>
       </c>
       <c r="D57">
-        <v>43.8</v>
+        <v>50</v>
       </c>
       <c r="E57">
         <v>12.5</v>
@@ -1987,7 +2041,7 @@
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2007,7 +2061,7 @@
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C59">
         <v>21.7</v>
@@ -2027,7 +2081,7 @@
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C60">
         <v>33.3</v>
@@ -2047,7 +2101,7 @@
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C61">
         <v>40</v>
@@ -2067,13 +2121,13 @@
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C62">
-        <v>13</v>
+        <v>15.3</v>
       </c>
       <c r="D62">
-        <v>18.7</v>
+        <v>20.8</v>
       </c>
       <c r="E62">
         <v>0.5</v>
@@ -2087,7 +2141,7 @@
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C63">
         <v>25</v>
@@ -2107,7 +2161,7 @@
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C64">
         <v>41.7</v>
@@ -2127,13 +2181,13 @@
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C65">
         <v>23.3</v>
       </c>
       <c r="D65">
-        <v>26.7</v>
+        <v>30</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2147,7 +2201,7 @@
         <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2167,13 +2221,13 @@
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C67">
-        <v>6.7</v>
+        <v>13.3</v>
       </c>
       <c r="D67">
-        <v>26.7</v>
+        <v>33.3</v>
       </c>
       <c r="E67">
         <v>6.7</v>
@@ -2187,7 +2241,7 @@
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C68">
         <v>40</v>
@@ -2207,7 +2261,7 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C69">
         <v>75</v>
@@ -2227,7 +2281,7 @@
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C70">
         <v>40</v>
@@ -2247,7 +2301,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C71">
         <v>50</v>
@@ -2267,13 +2321,13 @@
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C72">
-        <v>21.4</v>
+        <v>28.6</v>
       </c>
       <c r="D72">
-        <v>28.6</v>
+        <v>35.7</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -2287,7 +2341,7 @@
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C73">
         <v>75</v>
@@ -2307,7 +2361,7 @@
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C74">
         <v>18.2</v>
@@ -2327,10 +2381,10 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C75">
-        <v>30.8</v>
+        <v>38.5</v>
       </c>
       <c r="D75">
         <v>38.5</v>
@@ -2347,13 +2401,13 @@
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C76">
-        <v>5.3</v>
+        <v>10.5</v>
       </c>
       <c r="D76">
-        <v>31.6</v>
+        <v>36.8</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -2367,13 +2421,13 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>11.1</v>
       </c>
       <c r="D77">
-        <v>33.3</v>
+        <v>44.4</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -2387,13 +2441,13 @@
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C78">
         <v>20.7</v>
       </c>
       <c r="D78">
-        <v>37.9</v>
+        <v>34.5</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -2407,7 +2461,7 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C79">
         <v>11.1</v>
@@ -2427,7 +2481,7 @@
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2447,7 +2501,7 @@
         <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2467,13 +2521,13 @@
         <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C82">
-        <v>25</v>
+        <v>32.1</v>
       </c>
       <c r="D82">
-        <v>28.6</v>
+        <v>35.7</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -2487,13 +2541,13 @@
         <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C83">
-        <v>37.5</v>
+        <v>75</v>
       </c>
       <c r="D83">
-        <v>37.5</v>
+        <v>87.5</v>
       </c>
       <c r="E83">
         <v>12.5</v>
@@ -2507,13 +2561,13 @@
         <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>16.7</v>
       </c>
       <c r="D84">
-        <v>16.7</v>
+        <v>33.3</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -2527,7 +2581,7 @@
         <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C85">
         <v>10</v>
@@ -2547,7 +2601,7 @@
         <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C86">
         <v>29.4</v>
@@ -2567,13 +2621,13 @@
         <v>11</v>
       </c>
       <c r="B87" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C87">
-        <v>27.8</v>
+        <v>61.1</v>
       </c>
       <c r="D87">
-        <v>44.4</v>
+        <v>66.7</v>
       </c>
       <c r="E87">
         <v>5.6</v>
@@ -2587,13 +2641,13 @@
         <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C88">
         <v>16</v>
       </c>
       <c r="D88">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -2607,13 +2661,13 @@
         <v>11</v>
       </c>
       <c r="B89" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C89">
-        <v>21</v>
+        <v>26.3</v>
       </c>
       <c r="D89">
-        <v>34.7</v>
+        <v>39.8</v>
       </c>
       <c r="E89">
         <v>1.2</v>
@@ -2627,7 +2681,7 @@
         <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C90">
         <v>50</v>
@@ -2647,10 +2701,10 @@
         <v>11</v>
       </c>
       <c r="B91" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C91">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D91">
         <v>20</v>
@@ -2667,13 +2721,13 @@
         <v>11</v>
       </c>
       <c r="B92" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C92">
-        <v>9.1</v>
+        <v>54.5</v>
       </c>
       <c r="D92">
-        <v>9.1</v>
+        <v>63.6</v>
       </c>
       <c r="E92">
         <v>9.1</v>
@@ -2687,10 +2741,10 @@
         <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C93">
-        <v>33.3</v>
+        <v>50</v>
       </c>
       <c r="D93">
         <v>33.3</v>
@@ -2707,13 +2761,13 @@
         <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C94">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D94">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -2727,13 +2781,13 @@
         <v>11</v>
       </c>
       <c r="B95" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C95">
-        <v>18.3</v>
+        <v>23.3</v>
       </c>
       <c r="D95">
-        <v>23.3</v>
+        <v>28.3</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -2747,7 +2801,7 @@
         <v>11</v>
       </c>
       <c r="B96" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -2767,7 +2821,7 @@
         <v>11</v>
       </c>
       <c r="B97" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C97">
         <v>66.7</v>
@@ -2787,7 +2841,7 @@
         <v>11</v>
       </c>
       <c r="B98" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C98">
         <v>30</v>
@@ -2807,7 +2861,7 @@
         <v>11</v>
       </c>
       <c r="B99" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C99">
         <v>40</v>
@@ -2827,13 +2881,13 @@
         <v>11</v>
       </c>
       <c r="B100" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C100">
-        <v>21.4</v>
+        <v>28.6</v>
       </c>
       <c r="D100">
-        <v>21.4</v>
+        <v>28.6</v>
       </c>
       <c r="E100">
         <v>0</v>
@@ -2847,13 +2901,13 @@
         <v>11</v>
       </c>
       <c r="B101" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C101">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D101">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E101">
         <v>0</v>
@@ -2867,7 +2921,7 @@
         <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C102">
         <v>40</v>
@@ -2887,13 +2941,13 @@
         <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C103">
         <v>20.9</v>
       </c>
       <c r="D103">
-        <v>16.3</v>
+        <v>18.6</v>
       </c>
       <c r="E103">
         <v>2.3</v>
@@ -2907,7 +2961,7 @@
         <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C104">
         <v>26.3</v>
@@ -2927,7 +2981,7 @@
         <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -2947,13 +3001,13 @@
         <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C106">
-        <v>25.4</v>
+        <v>26.9</v>
       </c>
       <c r="D106">
-        <v>28.4</v>
+        <v>32.8</v>
       </c>
       <c r="E106">
         <v>0</v>
@@ -2967,13 +3021,13 @@
         <v>11</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C107">
-        <v>25</v>
+        <v>31.2</v>
       </c>
       <c r="D107">
-        <v>46.9</v>
+        <v>56.2</v>
       </c>
       <c r="E107">
         <v>0</v>
@@ -2987,13 +3041,13 @@
         <v>11</v>
       </c>
       <c r="B108" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C108">
-        <v>22.2</v>
+        <v>33.3</v>
       </c>
       <c r="D108">
-        <v>27.8</v>
+        <v>38.9</v>
       </c>
       <c r="E108">
         <v>0</v>
@@ -3007,13 +3061,13 @@
         <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C109">
-        <v>33.3</v>
+        <v>26.7</v>
       </c>
       <c r="D109">
-        <v>53.3</v>
+        <v>46.7</v>
       </c>
       <c r="E109">
         <v>0</v>
@@ -3027,7 +3081,7 @@
         <v>11</v>
       </c>
       <c r="B110" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C110">
         <v>25</v>
@@ -3047,7 +3101,7 @@
         <v>11</v>
       </c>
       <c r="B111" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C111">
         <v>22.6</v>
@@ -3067,7 +3121,7 @@
         <v>11</v>
       </c>
       <c r="B112" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -3087,7 +3141,7 @@
         <v>11</v>
       </c>
       <c r="B113" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C113">
         <v>60</v>
@@ -3107,13 +3161,13 @@
         <v>11</v>
       </c>
       <c r="B114" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C114">
         <v>31.8</v>
       </c>
       <c r="D114">
-        <v>50</v>
+        <v>45.5</v>
       </c>
       <c r="E114">
         <v>4.5</v>
@@ -3127,7 +3181,7 @@
         <v>11</v>
       </c>
       <c r="B115" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C115">
         <v>25</v>
@@ -3147,13 +3201,13 @@
         <v>11</v>
       </c>
       <c r="B116" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C116">
         <v>22.7</v>
       </c>
       <c r="D116">
-        <v>36.4</v>
+        <v>31.8</v>
       </c>
       <c r="E116">
         <v>0</v>
@@ -3167,13 +3221,13 @@
         <v>11</v>
       </c>
       <c r="B117" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C117">
-        <v>10.5</v>
+        <v>15.8</v>
       </c>
       <c r="D117">
-        <v>21.1</v>
+        <v>26.3</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -3187,7 +3241,7 @@
         <v>11</v>
       </c>
       <c r="B118" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C118">
         <v>28.6</v>
@@ -3207,13 +3261,13 @@
         <v>11</v>
       </c>
       <c r="B119" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C119">
-        <v>14.3</v>
+        <v>28.6</v>
       </c>
       <c r="D119">
-        <v>14.3</v>
+        <v>35.7</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -3227,13 +3281,13 @@
         <v>11</v>
       </c>
       <c r="B120" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C120">
-        <v>22.2</v>
+        <v>27.8</v>
       </c>
       <c r="D120">
-        <v>30.6</v>
+        <v>36.1</v>
       </c>
       <c r="E120">
         <v>5.6</v>
@@ -3247,13 +3301,13 @@
         <v>11</v>
       </c>
       <c r="B121" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="D121">
-        <v>18.2</v>
+        <v>27.3</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -3267,13 +3321,13 @@
         <v>11</v>
       </c>
       <c r="B122" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C122">
-        <v>12.5</v>
+        <v>25</v>
       </c>
       <c r="D122">
-        <v>25</v>
+        <v>37.5</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -3287,7 +3341,7 @@
         <v>11</v>
       </c>
       <c r="B123" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C123">
         <v>35.9</v>
@@ -3307,7 +3361,7 @@
         <v>11</v>
       </c>
       <c r="B124" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C124">
         <v>25</v>
@@ -3327,13 +3381,13 @@
         <v>11</v>
       </c>
       <c r="B125" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D125">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E125">
         <v>10</v>
@@ -3347,7 +3401,7 @@
         <v>11</v>
       </c>
       <c r="B126" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C126">
         <v>50</v>
@@ -3367,13 +3421,13 @@
         <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C127">
-        <v>13.3</v>
+        <v>40</v>
       </c>
       <c r="D127">
-        <v>20</v>
+        <v>46.7</v>
       </c>
       <c r="E127">
         <v>0</v>
@@ -3387,7 +3441,7 @@
         <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C128">
         <v>40</v>
@@ -3407,7 +3461,7 @@
         <v>11</v>
       </c>
       <c r="B129" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C129">
         <v>14.3</v>
@@ -3427,7 +3481,7 @@
         <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C130">
         <v>13.3</v>
@@ -3447,7 +3501,7 @@
         <v>11</v>
       </c>
       <c r="B131" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C131">
         <v>11.1</v>
@@ -3467,7 +3521,7 @@
         <v>11</v>
       </c>
       <c r="B132" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C132">
         <v>21.6</v>
@@ -3487,13 +3541,13 @@
         <v>11</v>
       </c>
       <c r="B133" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C133">
         <v>12</v>
       </c>
       <c r="D133">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E133">
         <v>0</v>
@@ -3507,7 +3561,7 @@
         <v>11</v>
       </c>
       <c r="B134" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C134">
         <v>28.6</v>
@@ -3527,13 +3581,13 @@
         <v>11</v>
       </c>
       <c r="B135" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C135">
-        <v>16.5</v>
+        <v>17.4</v>
       </c>
       <c r="D135">
-        <v>27.5</v>
+        <v>29.4</v>
       </c>
       <c r="E135">
         <v>0.9</v>
@@ -3547,7 +3601,7 @@
         <v>11</v>
       </c>
       <c r="B136" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -3567,13 +3621,13 @@
         <v>11</v>
       </c>
       <c r="B137" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C137">
-        <v>10.3</v>
+        <v>13.8</v>
       </c>
       <c r="D137">
-        <v>41.4</v>
+        <v>44.8</v>
       </c>
       <c r="E137">
         <v>0</v>
@@ -3587,13 +3641,13 @@
         <v>11</v>
       </c>
       <c r="B138" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C138">
-        <v>25.4</v>
+        <v>28.6</v>
       </c>
       <c r="D138">
-        <v>39.7</v>
+        <v>42.9</v>
       </c>
       <c r="E138">
         <v>0</v>
@@ -3607,7 +3661,7 @@
         <v>11</v>
       </c>
       <c r="B139" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -3627,13 +3681,13 @@
         <v>11</v>
       </c>
       <c r="B140" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C140">
-        <v>12.3</v>
+        <v>13.8</v>
       </c>
       <c r="D140">
-        <v>26.2</v>
+        <v>30.8</v>
       </c>
       <c r="E140">
         <v>1.5</v>
@@ -3647,10 +3701,10 @@
         <v>11</v>
       </c>
       <c r="B141" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C141">
-        <v>15.6</v>
+        <v>21.9</v>
       </c>
       <c r="D141">
         <v>28.1</v>
@@ -3667,13 +3721,13 @@
         <v>11</v>
       </c>
       <c r="B142" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C142">
-        <v>37.5</v>
+        <v>40.6</v>
       </c>
       <c r="D142">
-        <v>43.8</v>
+        <v>46.9</v>
       </c>
       <c r="E142">
         <v>6.2</v>
@@ -3687,7 +3741,7 @@
         <v>11</v>
       </c>
       <c r="B143" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C143">
         <v>6.7</v>
@@ -3707,7 +3761,7 @@
         <v>11</v>
       </c>
       <c r="B144" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C144">
         <v>50</v>
@@ -3727,19 +3781,439 @@
         <v>11</v>
       </c>
       <c r="B145" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C145">
-        <v>20.8</v>
+        <v>22.8</v>
       </c>
       <c r="D145">
-        <v>30.7</v>
+        <v>34.7</v>
       </c>
       <c r="E145">
         <v>0</v>
       </c>
       <c r="F145">
         <v>101</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" t="s">
+        <v>50</v>
+      </c>
+      <c r="C146">
+        <v>28.6</v>
+      </c>
+      <c r="D146">
+        <v>35.2</v>
+      </c>
+      <c r="E146">
+        <v>2.2</v>
+      </c>
+      <c r="F146">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" t="s">
+        <v>12</v>
+      </c>
+      <c r="B147" t="s">
+        <v>156</v>
+      </c>
+      <c r="C147">
+        <v>20.8</v>
+      </c>
+      <c r="D147">
+        <v>22.9</v>
+      </c>
+      <c r="E147">
+        <v>0.8</v>
+      </c>
+      <c r="F147">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" t="s">
+        <v>12</v>
+      </c>
+      <c r="B148" t="s">
+        <v>157</v>
+      </c>
+      <c r="C148">
+        <v>27.1</v>
+      </c>
+      <c r="D148">
+        <v>41.7</v>
+      </c>
+      <c r="E148">
+        <v>3.1</v>
+      </c>
+      <c r="F148">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" t="s">
+        <v>12</v>
+      </c>
+      <c r="B149" t="s">
+        <v>158</v>
+      </c>
+      <c r="C149">
+        <v>19.2</v>
+      </c>
+      <c r="D149">
+        <v>25</v>
+      </c>
+      <c r="E149">
+        <v>0.7</v>
+      </c>
+      <c r="F149">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" t="s">
+        <v>12</v>
+      </c>
+      <c r="B150" t="s">
+        <v>159</v>
+      </c>
+      <c r="C150">
+        <v>30.8</v>
+      </c>
+      <c r="D150">
+        <v>23.1</v>
+      </c>
+      <c r="E150">
+        <v>7.7</v>
+      </c>
+      <c r="F150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" t="s">
+        <v>12</v>
+      </c>
+      <c r="B151" t="s">
+        <v>82</v>
+      </c>
+      <c r="C151">
+        <v>28.6</v>
+      </c>
+      <c r="D151">
+        <v>35.7</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" t="s">
+        <v>12</v>
+      </c>
+      <c r="B152" t="s">
+        <v>160</v>
+      </c>
+      <c r="C152">
+        <v>20.7</v>
+      </c>
+      <c r="D152">
+        <v>35.3</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" t="s">
+        <v>12</v>
+      </c>
+      <c r="B153" t="s">
+        <v>161</v>
+      </c>
+      <c r="C153">
+        <v>33.3</v>
+      </c>
+      <c r="D153">
+        <v>46.4</v>
+      </c>
+      <c r="E153">
+        <v>2.4</v>
+      </c>
+      <c r="F153">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" t="s">
+        <v>12</v>
+      </c>
+      <c r="B154" t="s">
+        <v>99</v>
+      </c>
+      <c r="C154">
+        <v>26.3</v>
+      </c>
+      <c r="D154">
+        <v>39.8</v>
+      </c>
+      <c r="E154">
+        <v>1.2</v>
+      </c>
+      <c r="F154">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" t="s">
+        <v>12</v>
+      </c>
+      <c r="B155" t="s">
+        <v>162</v>
+      </c>
+      <c r="C155">
+        <v>45.5</v>
+      </c>
+      <c r="D155">
+        <v>39.4</v>
+      </c>
+      <c r="E155">
+        <v>3</v>
+      </c>
+      <c r="F155">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" t="s">
+        <v>12</v>
+      </c>
+      <c r="B156" t="s">
+        <v>163</v>
+      </c>
+      <c r="C156">
+        <v>16.9</v>
+      </c>
+      <c r="D156">
+        <v>19.9</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" t="s">
+        <v>12</v>
+      </c>
+      <c r="B157" t="s">
+        <v>164</v>
+      </c>
+      <c r="C157">
+        <v>31.9</v>
+      </c>
+      <c r="D157">
+        <v>38.3</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" t="s">
+        <v>12</v>
+      </c>
+      <c r="B158" t="s">
+        <v>113</v>
+      </c>
+      <c r="C158">
+        <v>20.9</v>
+      </c>
+      <c r="D158">
+        <v>18.6</v>
+      </c>
+      <c r="E158">
+        <v>2.3</v>
+      </c>
+      <c r="F158">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" t="s">
+        <v>12</v>
+      </c>
+      <c r="B159" t="s">
+        <v>165</v>
+      </c>
+      <c r="C159">
+        <v>26.3</v>
+      </c>
+      <c r="D159">
+        <v>37.1</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" t="s">
+        <v>12</v>
+      </c>
+      <c r="B160" t="s">
+        <v>166</v>
+      </c>
+      <c r="C160">
+        <v>24.3</v>
+      </c>
+      <c r="D160">
+        <v>38.7</v>
+      </c>
+      <c r="E160">
+        <v>1.8</v>
+      </c>
+      <c r="F160">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" t="s">
+        <v>12</v>
+      </c>
+      <c r="B161" t="s">
+        <v>167</v>
+      </c>
+      <c r="C161">
+        <v>28.6</v>
+      </c>
+      <c r="D161">
+        <v>33.3</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+      <c r="F161">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" t="s">
+        <v>12</v>
+      </c>
+      <c r="B162" t="s">
+        <v>168</v>
+      </c>
+      <c r="C162">
+        <v>28.4</v>
+      </c>
+      <c r="D162">
+        <v>36.3</v>
+      </c>
+      <c r="E162">
+        <v>2.9</v>
+      </c>
+      <c r="F162">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" t="s">
+        <v>12</v>
+      </c>
+      <c r="B163" t="s">
+        <v>169</v>
+      </c>
+      <c r="C163">
+        <v>32.4</v>
+      </c>
+      <c r="D163">
+        <v>41.2</v>
+      </c>
+      <c r="E163">
+        <v>2.9</v>
+      </c>
+      <c r="F163">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" t="s">
+        <v>12</v>
+      </c>
+      <c r="B164" t="s">
+        <v>170</v>
+      </c>
+      <c r="C164">
+        <v>17</v>
+      </c>
+      <c r="D164">
+        <v>30.8</v>
+      </c>
+      <c r="E164">
+        <v>0.4</v>
+      </c>
+      <c r="F164">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" t="s">
+        <v>12</v>
+      </c>
+      <c r="B165" t="s">
+        <v>171</v>
+      </c>
+      <c r="C165">
+        <v>12.1</v>
+      </c>
+      <c r="D165">
+        <v>42.4</v>
+      </c>
+      <c r="E165">
+        <v>0</v>
+      </c>
+      <c r="F165">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" t="s">
+        <v>12</v>
+      </c>
+      <c r="B166" t="s">
+        <v>172</v>
+      </c>
+      <c r="C166">
+        <v>23.5</v>
+      </c>
+      <c r="D166">
+        <v>34.9</v>
+      </c>
+      <c r="E166">
+        <v>0.9</v>
+      </c>
+      <c r="F166">
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>